<commit_message>
deleted Health and Social Sci
</commit_message>
<xml_diff>
--- a/Degrees_at_University/data/test_data_file.xlsx
+++ b/Degrees_at_University/data/test_data_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianeshomefolder/Documents/git/Brute-Force-Grad-College-Rankings-Map/Degrees_at_University/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3C0484-82FE-6B4E-BCFC-BE90DC142032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A085FA0A-AAC0-7C44-ACC4-015990D54976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="16100" xr2:uid="{66527176-1C23-DD43-B7D9-88C3EB420C4C}"/>
+    <workbookView xWindow="0" yWindow="960" windowWidth="27640" windowHeight="16100" xr2:uid="{66527176-1C23-DD43-B7D9-88C3EB420C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="272">
   <si>
     <t>Yale University</t>
   </si>
@@ -522,13 +522,340 @@
   </si>
   <si>
     <t>Engineering</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Johns Hopkins University</t>
+  </si>
+  <si>
+    <t>3400 N Charles St</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>21218-2688</t>
+  </si>
+  <si>
+    <t>BALTIMORE CITY</t>
+  </si>
+  <si>
+    <t>Baltimore-Columbia-Towson, MD</t>
+  </si>
+  <si>
+    <t>Washington-Baltimore-Arlington, DC-MD-VA-WV-PA</t>
+  </si>
+  <si>
+    <t>Nursing</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>University of California-Los Angeles</t>
+  </si>
+  <si>
+    <t>405 Hilgard Ave</t>
+  </si>
+  <si>
+    <t>90095-1405</t>
+  </si>
+  <si>
+    <t>University of Wisconsin-Madison</t>
+  </si>
+  <si>
+    <t>500 Lincoln Dr</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>53706-1380</t>
+  </si>
+  <si>
+    <t>DANE COUNTY</t>
+  </si>
+  <si>
+    <t>Madison, WI</t>
+  </si>
+  <si>
+    <t>Madison-Janesville-Beloit, WI</t>
+  </si>
+  <si>
+    <t>Vanderbilt University</t>
+  </si>
+  <si>
+    <t>2101 West End Avenue</t>
+  </si>
+  <si>
+    <t>Nashville</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>DAVIDSON COUNTY</t>
+  </si>
+  <si>
+    <t>Nashville-Davidson--Murfreesboro--Franklin, TN</t>
+  </si>
+  <si>
+    <t>Nashville-Davidson--Murfreesboro, TN</t>
+  </si>
+  <si>
+    <t>Fine Arts</t>
+  </si>
+  <si>
+    <t>Virginia Commonwealth University</t>
+  </si>
+  <si>
+    <t>910 W Franklin St</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>23284-2512</t>
+  </si>
+  <si>
+    <t>RICHMOND CITY</t>
+  </si>
+  <si>
+    <t>Richmond, VA</t>
+  </si>
+  <si>
+    <t>Rhode Island School of Design</t>
+  </si>
+  <si>
+    <t>2 College St</t>
+  </si>
+  <si>
+    <t>Providence</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>02903-2784</t>
+  </si>
+  <si>
+    <t>PROVIDENCE COUNTY</t>
+  </si>
+  <si>
+    <t>Providence-Warwick, RI-MA</t>
+  </si>
+  <si>
+    <t>School of the Art Institute of Chicago</t>
+  </si>
+  <si>
+    <t>36 S Wabash</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>University of Iowa</t>
+  </si>
+  <si>
+    <t>101 Jessup Hall</t>
+  </si>
+  <si>
+    <t>Iowa City</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>52242-1316</t>
+  </si>
+  <si>
+    <t>JOHNSON COUNTY</t>
+  </si>
+  <si>
+    <t>Iowa City, IA</t>
+  </si>
+  <si>
+    <t>Cedar Rapids-Iowa City, IA</t>
+  </si>
+  <si>
+    <t>Washington University in St Louis</t>
+  </si>
+  <si>
+    <t>One Brookings Drive</t>
+  </si>
+  <si>
+    <t>Saint Louis</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>63130-4899</t>
+  </si>
+  <si>
+    <t>ST. LOUIS COUNTY</t>
+  </si>
+  <si>
+    <t>St. Louis, MO-IL</t>
+  </si>
+  <si>
+    <t>St. Louis-St. Charles-Farmington, MO-IL</t>
+  </si>
+  <si>
+    <t>University of North Carolina at Chapel Hill</t>
+  </si>
+  <si>
+    <t>103 South Bldg Cb 9100</t>
+  </si>
+  <si>
+    <t>Chapel Hill</t>
+  </si>
+  <si>
+    <t>ORANGE COUNTY</t>
+  </si>
+  <si>
+    <t>The University of Texas at Dallas</t>
+  </si>
+  <si>
+    <t>800 West Campbell  Road</t>
+  </si>
+  <si>
+    <t>Richardson</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>75080-3021</t>
+  </si>
+  <si>
+    <t>DALLAS COUNTY</t>
+  </si>
+  <si>
+    <t>Dallas-Fort Worth-Arlington, TX</t>
+  </si>
+  <si>
+    <t>Dallas-Fort Worth, TX-OK</t>
+  </si>
+  <si>
+    <t>University of Washington-Seattle Campus</t>
+  </si>
+  <si>
+    <t>1400 NE Campus Parkway</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>98195-4550</t>
+  </si>
+  <si>
+    <t>KING COUNTY</t>
+  </si>
+  <si>
+    <t>Seattle-Tacoma-Bellevue, WA</t>
+  </si>
+  <si>
+    <t>Seattle-Tacoma, WA</t>
+  </si>
+  <si>
+    <t>Library and Information Studies</t>
+  </si>
+  <si>
+    <t>Indiana University-Bloomington</t>
+  </si>
+  <si>
+    <t>107 South Indiana Ave.</t>
+  </si>
+  <si>
+    <t>Bloomington</t>
+  </si>
+  <si>
+    <t>47405-7000</t>
+  </si>
+  <si>
+    <t>MONROE COUNTY</t>
+  </si>
+  <si>
+    <t>Bloomington, IN</t>
+  </si>
+  <si>
+    <t>Bloomington-Bedford, IN</t>
+  </si>
+  <si>
+    <t>Public Affairs</t>
+  </si>
+  <si>
+    <t>Syracuse University</t>
+  </si>
+  <si>
+    <t>900 South Crouse Ave.</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>ONONDAGA COUNTY</t>
+  </si>
+  <si>
+    <t>Syracuse, NY</t>
+  </si>
+  <si>
+    <t>Syracuse-Auburn, NY</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>University of Maryland-College Park</t>
+  </si>
+  <si>
+    <t>College Park</t>
+  </si>
+  <si>
+    <t>PRINCE GEORGE'S COUNTY</t>
+  </si>
+  <si>
+    <t>Washington-Arlington-Alexandria, DC-VA-MD-WV</t>
+  </si>
+  <si>
+    <t>Social Sciences and Humanities</t>
+  </si>
+  <si>
+    <t>SUNY at Albany</t>
+  </si>
+  <si>
+    <t>1400 Washington Avenue</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>ALBANY COUNTY</t>
+  </si>
+  <si>
+    <t>Albany-Schenectady-Troy, NY</t>
+  </si>
+  <si>
+    <t>Albany-Schenectady, NY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -564,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -572,6 +899,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,13 +1225,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C19401-FBE5-4745-AB86-FBFE0CC5B66A}">
-  <dimension ref="A1:AB38"/>
+  <dimension ref="A1:AB74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="5.83203125" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" customWidth="1"/>
@@ -908,11 +1247,11 @@
     <col min="23" max="23" width="5.6640625" customWidth="1"/>
     <col min="24" max="25" width="6.5" customWidth="1"/>
     <col min="26" max="26" width="10.1640625" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="12.83203125" style="5" customWidth="1"/>
     <col min="28" max="28" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -991,14 +1330,14 @@
       <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="5" t="s">
         <v>161</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-72.926689139999993</v>
       </c>
@@ -1077,14 +1416,14 @@
       <c r="Z2">
         <v>2016</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-122.1644471</v>
       </c>
@@ -1163,14 +1502,14 @@
       <c r="Z3">
         <v>2016</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AA3" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-71.118313610000001</v>
       </c>
@@ -1249,14 +1588,14 @@
       <c r="Z4">
         <v>2016</v>
       </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AA4" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-87.60120173</v>
       </c>
@@ -1335,14 +1674,14 @@
       <c r="Z5">
         <v>2016</v>
       </c>
-      <c r="AA5" s="2" t="s">
+      <c r="AA5" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-73.961886440000001</v>
       </c>
@@ -1421,14 +1760,14 @@
       <c r="Z6">
         <v>2016</v>
       </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AA6" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-73.99726545</v>
       </c>
@@ -1507,14 +1846,14 @@
       <c r="Z7">
         <v>2016</v>
       </c>
-      <c r="AA7" s="2" t="s">
+      <c r="AA7" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-75.193911779999993</v>
       </c>
@@ -1593,14 +1932,14 @@
       <c r="Z8">
         <v>2016</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AA8" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-78.503430699999996</v>
       </c>
@@ -1679,14 +2018,14 @@
       <c r="Z9">
         <v>2016</v>
       </c>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-83.742773619999994</v>
       </c>
@@ -1765,14 +2104,14 @@
       <c r="Z10">
         <v>2016</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-78.937626710000004</v>
       </c>
@@ -1851,14 +2190,14 @@
       <c r="Z11">
         <v>2016</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AA11" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-87.679863780000005</v>
       </c>
@@ -1937,14 +2276,14 @@
       <c r="Z12">
         <v>2016</v>
       </c>
-      <c r="AA12" s="2" t="s">
+      <c r="AA12" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB12" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-122.2604762</v>
       </c>
@@ -2023,14 +2362,14 @@
       <c r="Z13">
         <v>2016</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AA13" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB13" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-76.483086360000001</v>
       </c>
@@ -2109,14 +2448,14 @@
       <c r="Z14">
         <v>2016</v>
       </c>
-      <c r="AA14" s="2" t="s">
+      <c r="AA14" s="5" t="s">
         <v>99</v>
       </c>
       <c r="AB14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-75.193911779999993</v>
       </c>
@@ -2195,14 +2534,14 @@
       <c r="Z15">
         <v>2016</v>
       </c>
-      <c r="AA15" s="2" t="s">
+      <c r="AA15" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-122.1644471</v>
       </c>
@@ -2281,14 +2620,14 @@
       <c r="Z16">
         <v>2016</v>
       </c>
-      <c r="AA16" s="2" t="s">
+      <c r="AA16" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-71.118313610000001</v>
       </c>
@@ -2367,14 +2706,14 @@
       <c r="Z17">
         <v>2016</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="AA17" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB17" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-71.0921156</v>
       </c>
@@ -2453,14 +2792,14 @@
       <c r="Z18">
         <v>2016</v>
       </c>
-      <c r="AA18" s="2" t="s">
+      <c r="AA18" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB18" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-87.60120173</v>
       </c>
@@ -2539,14 +2878,14 @@
       <c r="Z19">
         <v>2016</v>
       </c>
-      <c r="AA19" s="2" t="s">
+      <c r="AA19" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB19" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-73.961886440000001</v>
       </c>
@@ -2625,14 +2964,14 @@
       <c r="Z20">
         <v>2016</v>
       </c>
-      <c r="AA20" s="2" t="s">
+      <c r="AA20" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB20" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-87.679863780000005</v>
       </c>
@@ -2711,14 +3050,14 @@
       <c r="Z21">
         <v>2016</v>
       </c>
-      <c r="AA21" s="2" t="s">
+      <c r="AA21" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB21" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-122.2604762</v>
       </c>
@@ -2797,14 +3136,14 @@
       <c r="Z22">
         <v>2016</v>
       </c>
-      <c r="AA22" s="2" t="s">
+      <c r="AA22" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB22" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-72.926689139999993</v>
       </c>
@@ -2883,14 +3222,14 @@
       <c r="Z23">
         <v>2016</v>
       </c>
-      <c r="AA23" s="2" t="s">
+      <c r="AA23" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB23" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-78.937626710000004</v>
       </c>
@@ -2969,14 +3308,14 @@
       <c r="Z24">
         <v>2016</v>
       </c>
-      <c r="AA24" s="2" t="s">
+      <c r="AA24" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB24" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>-83.742773619999994</v>
       </c>
@@ -3055,14 +3394,14 @@
       <c r="Z25">
         <v>2016</v>
       </c>
-      <c r="AA25" s="2" t="s">
+      <c r="AA25" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB25" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-72.289950079999997</v>
       </c>
@@ -3141,14 +3480,14 @@
       <c r="Z26">
         <v>2016</v>
       </c>
-      <c r="AA26" s="2" t="s">
+      <c r="AA26" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB26" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-73.99726545</v>
       </c>
@@ -3227,14 +3566,14 @@
       <c r="Z27">
         <v>2016</v>
       </c>
-      <c r="AA27" s="2" t="s">
+      <c r="AA27" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB27" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-78.503430699999996</v>
       </c>
@@ -3313,14 +3652,14 @@
       <c r="Z28">
         <v>2016</v>
       </c>
-      <c r="AA28" s="2" t="s">
+      <c r="AA28" s="5" t="s">
         <v>111</v>
       </c>
       <c r="AB28" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-71.0921156</v>
       </c>
@@ -3399,14 +3738,14 @@
       <c r="Z29">
         <v>2016</v>
       </c>
-      <c r="AA29" s="2" t="s">
+      <c r="AA29" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB29" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-122.1644471</v>
       </c>
@@ -3485,14 +3824,14 @@
       <c r="Z30">
         <v>2016</v>
       </c>
-      <c r="AA30" s="2" t="s">
+      <c r="AA30" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB30" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-122.2604762</v>
       </c>
@@ -3571,14 +3910,14 @@
       <c r="Z31">
         <v>2016</v>
       </c>
-      <c r="AA31" s="2" t="s">
+      <c r="AA31" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB31" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-79.942917300000005</v>
       </c>
@@ -3657,14 +3996,14 @@
       <c r="Z32">
         <v>2016</v>
       </c>
-      <c r="AA32" s="2" t="s">
+      <c r="AA32" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB32" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-118.12575219999999</v>
       </c>
@@ -3743,14 +4082,14 @@
       <c r="Z33">
         <v>2016</v>
       </c>
-      <c r="AA33" s="2" t="s">
+      <c r="AA33" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB33" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-83.742773619999994</v>
       </c>
@@ -3829,14 +4168,14 @@
       <c r="Z34">
         <v>2016</v>
       </c>
-      <c r="AA34" s="2" t="s">
+      <c r="AA34" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB34" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-84.394836209999994</v>
       </c>
@@ -3915,14 +4254,14 @@
       <c r="Z35">
         <v>2016</v>
       </c>
-      <c r="AA35" s="2" t="s">
+      <c r="AA35" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB35" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-86.914440400000004</v>
       </c>
@@ -4001,14 +4340,14 @@
       <c r="Z36">
         <v>2016</v>
       </c>
-      <c r="AA36" s="2" t="s">
+      <c r="AA36" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB36" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-118.28418120000001</v>
       </c>
@@ -4087,14 +4426,14 @@
       <c r="Z37">
         <v>2016</v>
       </c>
-      <c r="AA37" s="2" t="s">
+      <c r="AA37" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB37" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>-88.230315000000004</v>
       </c>
@@ -4173,11 +4512,3107 @@
       <c r="Z38" s="3">
         <v>2016</v>
       </c>
-      <c r="AA38" s="2" t="s">
+      <c r="AA38" s="5" t="s">
         <v>162</v>
       </c>
       <c r="AB38" s="2">
         <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>-71.118313610000001</v>
+      </c>
+      <c r="B39">
+        <v>42.374479669999999</v>
+      </c>
+      <c r="C39">
+        <v>1678</v>
+      </c>
+      <c r="D39">
+        <v>166027</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39">
+        <v>2138</v>
+      </c>
+      <c r="J39">
+        <v>25</v>
+      </c>
+      <c r="K39">
+        <v>25017</v>
+      </c>
+      <c r="L39" t="s">
+        <v>46</v>
+      </c>
+      <c r="M39">
+        <v>12</v>
+      </c>
+      <c r="N39">
+        <v>42.374471</v>
+      </c>
+      <c r="O39">
+        <v>-71.118313000000001</v>
+      </c>
+      <c r="P39">
+        <v>14460</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>47</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <v>148</v>
+      </c>
+      <c r="T39" t="s">
+        <v>48</v>
+      </c>
+      <c r="U39">
+        <v>71650</v>
+      </c>
+      <c r="V39" t="s">
+        <v>49</v>
+      </c>
+      <c r="W39">
+        <v>2505</v>
+      </c>
+      <c r="X39">
+        <v>25142</v>
+      </c>
+      <c r="Y39">
+        <v>25026</v>
+      </c>
+      <c r="Z39">
+        <v>2016</v>
+      </c>
+      <c r="AA39" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>-76.621597190000003</v>
+      </c>
+      <c r="B40">
+        <v>39.328984890000001</v>
+      </c>
+      <c r="C40">
+        <v>1587</v>
+      </c>
+      <c r="D40">
+        <v>162928</v>
+      </c>
+      <c r="E40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F40" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" t="s">
+        <v>166</v>
+      </c>
+      <c r="H40" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" t="s">
+        <v>168</v>
+      </c>
+      <c r="J40">
+        <v>24</v>
+      </c>
+      <c r="K40">
+        <v>24510</v>
+      </c>
+      <c r="L40" t="s">
+        <v>169</v>
+      </c>
+      <c r="M40">
+        <v>11</v>
+      </c>
+      <c r="N40">
+        <v>39.328977000000002</v>
+      </c>
+      <c r="O40">
+        <v>-76.621594999999999</v>
+      </c>
+      <c r="P40">
+        <v>12580</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>170</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <v>548</v>
+      </c>
+      <c r="T40" t="s">
+        <v>171</v>
+      </c>
+      <c r="U40" t="s">
+        <v>41</v>
+      </c>
+      <c r="V40" t="s">
+        <v>41</v>
+      </c>
+      <c r="W40">
+        <v>2407</v>
+      </c>
+      <c r="X40">
+        <v>24040</v>
+      </c>
+      <c r="Y40">
+        <v>24040</v>
+      </c>
+      <c r="Z40">
+        <v>2016</v>
+      </c>
+      <c r="AA40" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>-122.1644471</v>
+      </c>
+      <c r="B41">
+        <v>37.429536929999998</v>
+      </c>
+      <c r="C41">
+        <v>4248</v>
+      </c>
+      <c r="D41">
+        <v>243744</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41">
+        <v>94305</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+      <c r="K41">
+        <v>6085</v>
+      </c>
+      <c r="L41" t="s">
+        <v>38</v>
+      </c>
+      <c r="M41">
+        <v>21</v>
+      </c>
+      <c r="N41">
+        <v>37.429532000000002</v>
+      </c>
+      <c r="O41">
+        <v>-122.164434</v>
+      </c>
+      <c r="P41">
+        <v>41940</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>39</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>488</v>
+      </c>
+      <c r="T41" t="s">
+        <v>40</v>
+      </c>
+      <c r="U41" t="s">
+        <v>41</v>
+      </c>
+      <c r="V41" t="s">
+        <v>41</v>
+      </c>
+      <c r="W41">
+        <v>618</v>
+      </c>
+      <c r="X41">
+        <v>6024</v>
+      </c>
+      <c r="Y41">
+        <v>6013</v>
+      </c>
+      <c r="Z41">
+        <v>2016</v>
+      </c>
+      <c r="AA41" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB41" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>-75.193911779999993</v>
+      </c>
+      <c r="B42">
+        <v>39.950937060000001</v>
+      </c>
+      <c r="C42">
+        <v>3334</v>
+      </c>
+      <c r="D42">
+        <v>215062</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" t="s">
+        <v>70</v>
+      </c>
+      <c r="J42">
+        <v>42</v>
+      </c>
+      <c r="K42">
+        <v>42101</v>
+      </c>
+      <c r="L42" t="s">
+        <v>71</v>
+      </c>
+      <c r="M42">
+        <v>11</v>
+      </c>
+      <c r="N42">
+        <v>39.950929000000002</v>
+      </c>
+      <c r="O42">
+        <v>-75.193910000000002</v>
+      </c>
+      <c r="P42">
+        <v>37980</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>72</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <v>428</v>
+      </c>
+      <c r="T42" t="s">
+        <v>73</v>
+      </c>
+      <c r="U42" t="s">
+        <v>41</v>
+      </c>
+      <c r="V42" t="s">
+        <v>41</v>
+      </c>
+      <c r="W42">
+        <v>4202</v>
+      </c>
+      <c r="X42">
+        <v>42188</v>
+      </c>
+      <c r="Y42">
+        <v>42008</v>
+      </c>
+      <c r="Z42">
+        <v>2016</v>
+      </c>
+      <c r="AA42" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>-76.621597190000003</v>
+      </c>
+      <c r="B43">
+        <v>39.328984890000001</v>
+      </c>
+      <c r="C43">
+        <v>1587</v>
+      </c>
+      <c r="D43">
+        <v>162928</v>
+      </c>
+      <c r="E43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" t="s">
+        <v>166</v>
+      </c>
+      <c r="H43" t="s">
+        <v>167</v>
+      </c>
+      <c r="I43" t="s">
+        <v>168</v>
+      </c>
+      <c r="J43">
+        <v>24</v>
+      </c>
+      <c r="K43">
+        <v>24510</v>
+      </c>
+      <c r="L43" t="s">
+        <v>169</v>
+      </c>
+      <c r="M43">
+        <v>11</v>
+      </c>
+      <c r="N43">
+        <v>39.328977000000002</v>
+      </c>
+      <c r="O43">
+        <v>-76.621594999999999</v>
+      </c>
+      <c r="P43">
+        <v>12580</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>170</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>548</v>
+      </c>
+      <c r="T43" t="s">
+        <v>171</v>
+      </c>
+      <c r="U43" t="s">
+        <v>41</v>
+      </c>
+      <c r="V43" t="s">
+        <v>41</v>
+      </c>
+      <c r="W43">
+        <v>2407</v>
+      </c>
+      <c r="X43">
+        <v>24040</v>
+      </c>
+      <c r="Y43">
+        <v>24040</v>
+      </c>
+      <c r="Z43">
+        <v>2016</v>
+      </c>
+      <c r="AA43" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>-78.937626710000004</v>
+      </c>
+      <c r="B44">
+        <v>36.001142119999997</v>
+      </c>
+      <c r="C44">
+        <v>2684</v>
+      </c>
+      <c r="D44">
+        <v>198419</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44" t="s">
+        <v>91</v>
+      </c>
+      <c r="I44">
+        <v>27708</v>
+      </c>
+      <c r="J44">
+        <v>37</v>
+      </c>
+      <c r="K44">
+        <v>37063</v>
+      </c>
+      <c r="L44" t="s">
+        <v>92</v>
+      </c>
+      <c r="M44">
+        <v>11</v>
+      </c>
+      <c r="N44">
+        <v>36.001134999999998</v>
+      </c>
+      <c r="O44">
+        <v>-78.937624</v>
+      </c>
+      <c r="P44">
+        <v>20500</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>93</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>450</v>
+      </c>
+      <c r="T44" t="s">
+        <v>94</v>
+      </c>
+      <c r="U44" t="s">
+        <v>41</v>
+      </c>
+      <c r="V44" t="s">
+        <v>41</v>
+      </c>
+      <c r="W44">
+        <v>3701</v>
+      </c>
+      <c r="X44">
+        <v>37030</v>
+      </c>
+      <c r="Y44">
+        <v>37022</v>
+      </c>
+      <c r="Z44">
+        <v>2016</v>
+      </c>
+      <c r="AA44" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>-75.193911779999993</v>
+      </c>
+      <c r="B45">
+        <v>39.950937060000001</v>
+      </c>
+      <c r="C45">
+        <v>3334</v>
+      </c>
+      <c r="D45">
+        <v>215062</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45" t="s">
+        <v>69</v>
+      </c>
+      <c r="I45" t="s">
+        <v>70</v>
+      </c>
+      <c r="J45">
+        <v>42</v>
+      </c>
+      <c r="K45">
+        <v>42101</v>
+      </c>
+      <c r="L45" t="s">
+        <v>71</v>
+      </c>
+      <c r="M45">
+        <v>11</v>
+      </c>
+      <c r="N45">
+        <v>39.950929000000002</v>
+      </c>
+      <c r="O45">
+        <v>-75.193910000000002</v>
+      </c>
+      <c r="P45">
+        <v>37980</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>72</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>428</v>
+      </c>
+      <c r="T45" t="s">
+        <v>73</v>
+      </c>
+      <c r="U45" t="s">
+        <v>41</v>
+      </c>
+      <c r="V45" t="s">
+        <v>41</v>
+      </c>
+      <c r="W45">
+        <v>4202</v>
+      </c>
+      <c r="X45">
+        <v>42188</v>
+      </c>
+      <c r="Y45">
+        <v>42008</v>
+      </c>
+      <c r="Z45">
+        <v>2016</v>
+      </c>
+      <c r="AA45" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB45" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>-71.118313610000001</v>
+      </c>
+      <c r="B46">
+        <v>42.374479669999999</v>
+      </c>
+      <c r="C46">
+        <v>1678</v>
+      </c>
+      <c r="D46">
+        <v>166027</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G46" t="s">
+        <v>44</v>
+      </c>
+      <c r="H46" t="s">
+        <v>45</v>
+      </c>
+      <c r="I46">
+        <v>2138</v>
+      </c>
+      <c r="J46">
+        <v>25</v>
+      </c>
+      <c r="K46">
+        <v>25017</v>
+      </c>
+      <c r="L46" t="s">
+        <v>46</v>
+      </c>
+      <c r="M46">
+        <v>12</v>
+      </c>
+      <c r="N46">
+        <v>42.374471</v>
+      </c>
+      <c r="O46">
+        <v>-71.118313000000001</v>
+      </c>
+      <c r="P46">
+        <v>14460</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>47</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+      <c r="S46">
+        <v>148</v>
+      </c>
+      <c r="T46" t="s">
+        <v>48</v>
+      </c>
+      <c r="U46">
+        <v>71650</v>
+      </c>
+      <c r="V46" t="s">
+        <v>49</v>
+      </c>
+      <c r="W46">
+        <v>2505</v>
+      </c>
+      <c r="X46">
+        <v>25142</v>
+      </c>
+      <c r="Y46">
+        <v>25026</v>
+      </c>
+      <c r="Z46">
+        <v>2016</v>
+      </c>
+      <c r="AA46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>-75.193911779999993</v>
+      </c>
+      <c r="B47">
+        <v>39.950937060000001</v>
+      </c>
+      <c r="C47">
+        <v>3334</v>
+      </c>
+      <c r="D47">
+        <v>215062</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" t="s">
+        <v>70</v>
+      </c>
+      <c r="J47">
+        <v>42</v>
+      </c>
+      <c r="K47">
+        <v>42101</v>
+      </c>
+      <c r="L47" t="s">
+        <v>71</v>
+      </c>
+      <c r="M47">
+        <v>11</v>
+      </c>
+      <c r="N47">
+        <v>39.950929000000002</v>
+      </c>
+      <c r="O47">
+        <v>-75.193910000000002</v>
+      </c>
+      <c r="P47">
+        <v>37980</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>72</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <v>428</v>
+      </c>
+      <c r="T47" t="s">
+        <v>73</v>
+      </c>
+      <c r="U47" t="s">
+        <v>41</v>
+      </c>
+      <c r="V47" t="s">
+        <v>41</v>
+      </c>
+      <c r="W47">
+        <v>4202</v>
+      </c>
+      <c r="X47">
+        <v>42188</v>
+      </c>
+      <c r="Y47">
+        <v>42008</v>
+      </c>
+      <c r="Z47">
+        <v>2016</v>
+      </c>
+      <c r="AA47" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB47" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>-122.1644471</v>
+      </c>
+      <c r="B48">
+        <v>37.429536929999998</v>
+      </c>
+      <c r="C48">
+        <v>4248</v>
+      </c>
+      <c r="D48">
+        <v>243744</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48">
+        <v>94305</v>
+      </c>
+      <c r="J48">
+        <v>6</v>
+      </c>
+      <c r="K48">
+        <v>6085</v>
+      </c>
+      <c r="L48" t="s">
+        <v>38</v>
+      </c>
+      <c r="M48">
+        <v>21</v>
+      </c>
+      <c r="N48">
+        <v>37.429532000000002</v>
+      </c>
+      <c r="O48">
+        <v>-122.164434</v>
+      </c>
+      <c r="P48">
+        <v>41940</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>39</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <v>488</v>
+      </c>
+      <c r="T48" t="s">
+        <v>40</v>
+      </c>
+      <c r="U48" t="s">
+        <v>41</v>
+      </c>
+      <c r="V48" t="s">
+        <v>41</v>
+      </c>
+      <c r="W48">
+        <v>618</v>
+      </c>
+      <c r="X48">
+        <v>6024</v>
+      </c>
+      <c r="Y48">
+        <v>6013</v>
+      </c>
+      <c r="Z48">
+        <v>2016</v>
+      </c>
+      <c r="AA48" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB48" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>-118.4439132</v>
+      </c>
+      <c r="B49">
+        <v>34.068896850000002</v>
+      </c>
+      <c r="C49">
+        <v>250</v>
+      </c>
+      <c r="D49">
+        <v>110662</v>
+      </c>
+      <c r="E49" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" t="s">
+        <v>154</v>
+      </c>
+      <c r="H49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" t="s">
+        <v>176</v>
+      </c>
+      <c r="J49">
+        <v>6</v>
+      </c>
+      <c r="K49">
+        <v>6037</v>
+      </c>
+      <c r="L49" t="s">
+        <v>133</v>
+      </c>
+      <c r="M49">
+        <v>11</v>
+      </c>
+      <c r="N49">
+        <v>34.068891999999998</v>
+      </c>
+      <c r="O49">
+        <v>-118.443901</v>
+      </c>
+      <c r="P49">
+        <v>31080</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>134</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <v>348</v>
+      </c>
+      <c r="T49" t="s">
+        <v>135</v>
+      </c>
+      <c r="U49" t="s">
+        <v>41</v>
+      </c>
+      <c r="V49" t="s">
+        <v>41</v>
+      </c>
+      <c r="W49">
+        <v>633</v>
+      </c>
+      <c r="X49">
+        <v>6054</v>
+      </c>
+      <c r="Y49">
+        <v>6026</v>
+      </c>
+      <c r="Z49">
+        <v>2016</v>
+      </c>
+      <c r="AA49" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB49" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>-89.405362400000001</v>
+      </c>
+      <c r="B50">
+        <v>43.073865949999998</v>
+      </c>
+      <c r="C50">
+        <v>4151</v>
+      </c>
+      <c r="D50">
+        <v>240444</v>
+      </c>
+      <c r="E50" t="s">
+        <v>177</v>
+      </c>
+      <c r="F50" t="s">
+        <v>178</v>
+      </c>
+      <c r="G50" t="s">
+        <v>179</v>
+      </c>
+      <c r="H50" t="s">
+        <v>180</v>
+      </c>
+      <c r="I50" t="s">
+        <v>181</v>
+      </c>
+      <c r="J50">
+        <v>55</v>
+      </c>
+      <c r="K50">
+        <v>55025</v>
+      </c>
+      <c r="L50" t="s">
+        <v>182</v>
+      </c>
+      <c r="M50">
+        <v>12</v>
+      </c>
+      <c r="N50">
+        <v>43.073858000000001</v>
+      </c>
+      <c r="O50">
+        <v>-89.405355999999998</v>
+      </c>
+      <c r="P50">
+        <v>31540</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>183</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>357</v>
+      </c>
+      <c r="T50" t="s">
+        <v>184</v>
+      </c>
+      <c r="U50" t="s">
+        <v>41</v>
+      </c>
+      <c r="V50" t="s">
+        <v>41</v>
+      </c>
+      <c r="W50">
+        <v>5502</v>
+      </c>
+      <c r="X50">
+        <v>55077</v>
+      </c>
+      <c r="Y50">
+        <v>55026</v>
+      </c>
+      <c r="Z50">
+        <v>2016</v>
+      </c>
+      <c r="AA50" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB50" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>-86.803374039999994</v>
+      </c>
+      <c r="B51">
+        <v>36.14659683</v>
+      </c>
+      <c r="C51">
+        <v>3622</v>
+      </c>
+      <c r="D51">
+        <v>221999</v>
+      </c>
+      <c r="E51" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" t="s">
+        <v>186</v>
+      </c>
+      <c r="G51" t="s">
+        <v>187</v>
+      </c>
+      <c r="H51" t="s">
+        <v>188</v>
+      </c>
+      <c r="I51">
+        <v>37240</v>
+      </c>
+      <c r="J51">
+        <v>47</v>
+      </c>
+      <c r="K51">
+        <v>47037</v>
+      </c>
+      <c r="L51" t="s">
+        <v>189</v>
+      </c>
+      <c r="M51">
+        <v>11</v>
+      </c>
+      <c r="N51">
+        <v>36.146590000000003</v>
+      </c>
+      <c r="O51">
+        <v>-86.803369000000004</v>
+      </c>
+      <c r="P51">
+        <v>34980</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>190</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>400</v>
+      </c>
+      <c r="T51" t="s">
+        <v>191</v>
+      </c>
+      <c r="U51" t="s">
+        <v>41</v>
+      </c>
+      <c r="V51" t="s">
+        <v>41</v>
+      </c>
+      <c r="W51">
+        <v>4705</v>
+      </c>
+      <c r="X51">
+        <v>47055</v>
+      </c>
+      <c r="Y51">
+        <v>47021</v>
+      </c>
+      <c r="Z51">
+        <v>2016</v>
+      </c>
+      <c r="AA51" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB51" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>-72.926689139999993</v>
+      </c>
+      <c r="B52">
+        <v>41.311166409999998</v>
+      </c>
+      <c r="C52">
+        <v>688</v>
+      </c>
+      <c r="D52">
+        <v>130794</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H52" t="s">
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>6520</v>
+      </c>
+      <c r="J52">
+        <v>9</v>
+      </c>
+      <c r="K52">
+        <v>9009</v>
+      </c>
+      <c r="L52" t="s">
+        <v>4</v>
+      </c>
+      <c r="M52">
+        <v>12</v>
+      </c>
+      <c r="N52">
+        <v>41.311157999999999</v>
+      </c>
+      <c r="O52">
+        <v>-72.926687999999999</v>
+      </c>
+      <c r="P52">
+        <v>35300</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>5</v>
+      </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
+      <c r="S52">
+        <v>408</v>
+      </c>
+      <c r="T52" t="s">
+        <v>6</v>
+      </c>
+      <c r="U52">
+        <v>75700</v>
+      </c>
+      <c r="V52" t="s">
+        <v>7</v>
+      </c>
+      <c r="W52">
+        <v>903</v>
+      </c>
+      <c r="X52">
+        <v>9094</v>
+      </c>
+      <c r="Y52">
+        <v>9011</v>
+      </c>
+      <c r="Z52">
+        <v>2016</v>
+      </c>
+      <c r="AA52" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>-118.4439132</v>
+      </c>
+      <c r="B53">
+        <v>34.068896850000002</v>
+      </c>
+      <c r="C53">
+        <v>250</v>
+      </c>
+      <c r="D53">
+        <v>110662</v>
+      </c>
+      <c r="E53" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" t="s">
+        <v>175</v>
+      </c>
+      <c r="G53" t="s">
+        <v>154</v>
+      </c>
+      <c r="H53" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" t="s">
+        <v>176</v>
+      </c>
+      <c r="J53">
+        <v>6</v>
+      </c>
+      <c r="K53">
+        <v>6037</v>
+      </c>
+      <c r="L53" t="s">
+        <v>133</v>
+      </c>
+      <c r="M53">
+        <v>11</v>
+      </c>
+      <c r="N53">
+        <v>34.068891999999998</v>
+      </c>
+      <c r="O53">
+        <v>-118.443901</v>
+      </c>
+      <c r="P53">
+        <v>31080</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>134</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <v>348</v>
+      </c>
+      <c r="T53" t="s">
+        <v>135</v>
+      </c>
+      <c r="U53" t="s">
+        <v>41</v>
+      </c>
+      <c r="V53" t="s">
+        <v>41</v>
+      </c>
+      <c r="W53">
+        <v>633</v>
+      </c>
+      <c r="X53">
+        <v>6054</v>
+      </c>
+      <c r="Y53">
+        <v>6026</v>
+      </c>
+      <c r="Z53">
+        <v>2016</v>
+      </c>
+      <c r="AA53" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB53" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>-77.453599339999997</v>
+      </c>
+      <c r="B54">
+        <v>37.547638489999997</v>
+      </c>
+      <c r="C54">
+        <v>3956</v>
+      </c>
+      <c r="D54">
+        <v>234030</v>
+      </c>
+      <c r="E54" t="s">
+        <v>193</v>
+      </c>
+      <c r="F54" t="s">
+        <v>194</v>
+      </c>
+      <c r="G54" t="s">
+        <v>195</v>
+      </c>
+      <c r="H54" t="s">
+        <v>77</v>
+      </c>
+      <c r="I54" t="s">
+        <v>196</v>
+      </c>
+      <c r="J54">
+        <v>51</v>
+      </c>
+      <c r="K54">
+        <v>51760</v>
+      </c>
+      <c r="L54" t="s">
+        <v>197</v>
+      </c>
+      <c r="M54">
+        <v>12</v>
+      </c>
+      <c r="N54">
+        <v>37.547631000000003</v>
+      </c>
+      <c r="O54">
+        <v>-77.453597000000002</v>
+      </c>
+      <c r="P54">
+        <v>40060</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>198</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54" t="s">
+        <v>41</v>
+      </c>
+      <c r="T54" t="s">
+        <v>41</v>
+      </c>
+      <c r="U54" t="s">
+        <v>41</v>
+      </c>
+      <c r="V54" t="s">
+        <v>41</v>
+      </c>
+      <c r="W54">
+        <v>5104</v>
+      </c>
+      <c r="X54">
+        <v>51071</v>
+      </c>
+      <c r="Y54">
+        <v>51010</v>
+      </c>
+      <c r="Z54">
+        <v>2016</v>
+      </c>
+      <c r="AA54" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB54" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>-71.407692670000003</v>
+      </c>
+      <c r="B55">
+        <v>41.825943559999999</v>
+      </c>
+      <c r="C55">
+        <v>3427</v>
+      </c>
+      <c r="D55">
+        <v>217493</v>
+      </c>
+      <c r="E55" t="s">
+        <v>199</v>
+      </c>
+      <c r="F55" t="s">
+        <v>200</v>
+      </c>
+      <c r="G55" t="s">
+        <v>201</v>
+      </c>
+      <c r="H55" t="s">
+        <v>202</v>
+      </c>
+      <c r="I55" t="s">
+        <v>203</v>
+      </c>
+      <c r="J55">
+        <v>44</v>
+      </c>
+      <c r="K55">
+        <v>44007</v>
+      </c>
+      <c r="L55" t="s">
+        <v>204</v>
+      </c>
+      <c r="M55">
+        <v>12</v>
+      </c>
+      <c r="N55">
+        <v>41.825935000000001</v>
+      </c>
+      <c r="O55">
+        <v>-71.407691999999997</v>
+      </c>
+      <c r="P55">
+        <v>39300</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>205</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <v>148</v>
+      </c>
+      <c r="T55" t="s">
+        <v>48</v>
+      </c>
+      <c r="U55">
+        <v>77200</v>
+      </c>
+      <c r="V55" t="s">
+        <v>205</v>
+      </c>
+      <c r="W55">
+        <v>4401</v>
+      </c>
+      <c r="X55">
+        <v>44001</v>
+      </c>
+      <c r="Y55">
+        <v>44003</v>
+      </c>
+      <c r="Z55">
+        <v>2016</v>
+      </c>
+      <c r="AA55" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB55" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>-87.621416749999995</v>
+      </c>
+      <c r="B56">
+        <v>41.879653849999997</v>
+      </c>
+      <c r="C56">
+        <v>979</v>
+      </c>
+      <c r="D56">
+        <v>143048</v>
+      </c>
+      <c r="E56" t="s">
+        <v>206</v>
+      </c>
+      <c r="F56" t="s">
+        <v>207</v>
+      </c>
+      <c r="G56" t="s">
+        <v>52</v>
+      </c>
+      <c r="H56" t="s">
+        <v>53</v>
+      </c>
+      <c r="I56">
+        <v>60603</v>
+      </c>
+      <c r="J56">
+        <v>17</v>
+      </c>
+      <c r="K56">
+        <v>17031</v>
+      </c>
+      <c r="L56" t="s">
+        <v>54</v>
+      </c>
+      <c r="M56">
+        <v>11</v>
+      </c>
+      <c r="N56">
+        <v>41.879646000000001</v>
+      </c>
+      <c r="O56">
+        <v>-87.621410999999995</v>
+      </c>
+      <c r="P56">
+        <v>16980</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>55</v>
+      </c>
+      <c r="R56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>176</v>
+      </c>
+      <c r="T56" t="s">
+        <v>56</v>
+      </c>
+      <c r="U56" t="s">
+        <v>41</v>
+      </c>
+      <c r="V56" t="s">
+        <v>41</v>
+      </c>
+      <c r="W56">
+        <v>1707</v>
+      </c>
+      <c r="X56">
+        <v>17026</v>
+      </c>
+      <c r="Y56">
+        <v>17013</v>
+      </c>
+      <c r="Z56">
+        <v>2016</v>
+      </c>
+      <c r="AA56" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB56" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>-86.803374039999994</v>
+      </c>
+      <c r="B57">
+        <v>36.14659683</v>
+      </c>
+      <c r="C57">
+        <v>3622</v>
+      </c>
+      <c r="D57">
+        <v>221999</v>
+      </c>
+      <c r="E57" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" t="s">
+        <v>187</v>
+      </c>
+      <c r="H57" t="s">
+        <v>188</v>
+      </c>
+      <c r="I57">
+        <v>37240</v>
+      </c>
+      <c r="J57">
+        <v>47</v>
+      </c>
+      <c r="K57">
+        <v>47037</v>
+      </c>
+      <c r="L57" t="s">
+        <v>189</v>
+      </c>
+      <c r="M57">
+        <v>11</v>
+      </c>
+      <c r="N57">
+        <v>36.146590000000003</v>
+      </c>
+      <c r="O57">
+        <v>-86.803369000000004</v>
+      </c>
+      <c r="P57">
+        <v>34980</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>190</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>400</v>
+      </c>
+      <c r="T57" t="s">
+        <v>191</v>
+      </c>
+      <c r="U57" t="s">
+        <v>41</v>
+      </c>
+      <c r="V57" t="s">
+        <v>41</v>
+      </c>
+      <c r="W57">
+        <v>4705</v>
+      </c>
+      <c r="X57">
+        <v>47055</v>
+      </c>
+      <c r="Y57">
+        <v>47021</v>
+      </c>
+      <c r="Z57">
+        <v>2016</v>
+      </c>
+      <c r="AA57" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>-91.536431859999993</v>
+      </c>
+      <c r="B58">
+        <v>41.661942590000002</v>
+      </c>
+      <c r="C58">
+        <v>1284</v>
+      </c>
+      <c r="D58">
+        <v>153658</v>
+      </c>
+      <c r="E58" t="s">
+        <v>209</v>
+      </c>
+      <c r="F58" t="s">
+        <v>210</v>
+      </c>
+      <c r="G58" t="s">
+        <v>211</v>
+      </c>
+      <c r="H58" t="s">
+        <v>212</v>
+      </c>
+      <c r="I58" t="s">
+        <v>213</v>
+      </c>
+      <c r="J58">
+        <v>19</v>
+      </c>
+      <c r="K58">
+        <v>19103</v>
+      </c>
+      <c r="L58" t="s">
+        <v>214</v>
+      </c>
+      <c r="M58">
+        <v>13</v>
+      </c>
+      <c r="N58">
+        <v>41.661935</v>
+      </c>
+      <c r="O58">
+        <v>-91.536424999999994</v>
+      </c>
+      <c r="P58">
+        <v>26980</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>215</v>
+      </c>
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="S58">
+        <v>168</v>
+      </c>
+      <c r="T58" t="s">
+        <v>216</v>
+      </c>
+      <c r="U58" t="s">
+        <v>41</v>
+      </c>
+      <c r="V58" t="s">
+        <v>41</v>
+      </c>
+      <c r="W58">
+        <v>1902</v>
+      </c>
+      <c r="X58">
+        <v>19085</v>
+      </c>
+      <c r="Y58">
+        <v>19043</v>
+      </c>
+      <c r="Z58">
+        <v>2016</v>
+      </c>
+      <c r="AA58" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB58" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>-90.310610220000001</v>
+      </c>
+      <c r="B59">
+        <v>38.647936139999999</v>
+      </c>
+      <c r="C59">
+        <v>2107</v>
+      </c>
+      <c r="D59">
+        <v>179867</v>
+      </c>
+      <c r="E59" t="s">
+        <v>217</v>
+      </c>
+      <c r="F59" t="s">
+        <v>218</v>
+      </c>
+      <c r="G59" t="s">
+        <v>219</v>
+      </c>
+      <c r="H59" t="s">
+        <v>220</v>
+      </c>
+      <c r="I59" t="s">
+        <v>221</v>
+      </c>
+      <c r="J59">
+        <v>29</v>
+      </c>
+      <c r="K59">
+        <v>29189</v>
+      </c>
+      <c r="L59" t="s">
+        <v>222</v>
+      </c>
+      <c r="M59">
+        <v>21</v>
+      </c>
+      <c r="N59">
+        <v>38.647928999999998</v>
+      </c>
+      <c r="O59">
+        <v>-90.310603999999998</v>
+      </c>
+      <c r="P59">
+        <v>41180</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>223</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>476</v>
+      </c>
+      <c r="T59" t="s">
+        <v>224</v>
+      </c>
+      <c r="U59" t="s">
+        <v>41</v>
+      </c>
+      <c r="V59" t="s">
+        <v>41</v>
+      </c>
+      <c r="W59">
+        <v>2901</v>
+      </c>
+      <c r="X59">
+        <v>29087</v>
+      </c>
+      <c r="Y59">
+        <v>29014</v>
+      </c>
+      <c r="Z59">
+        <v>2016</v>
+      </c>
+      <c r="AA59" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB59" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>-79.050971739999994</v>
+      </c>
+      <c r="B60">
+        <v>35.911776089999996</v>
+      </c>
+      <c r="C60">
+        <v>2731</v>
+      </c>
+      <c r="D60">
+        <v>199120</v>
+      </c>
+      <c r="E60" t="s">
+        <v>225</v>
+      </c>
+      <c r="F60" t="s">
+        <v>226</v>
+      </c>
+      <c r="G60" t="s">
+        <v>227</v>
+      </c>
+      <c r="H60" t="s">
+        <v>91</v>
+      </c>
+      <c r="I60">
+        <v>27599</v>
+      </c>
+      <c r="J60">
+        <v>37</v>
+      </c>
+      <c r="K60">
+        <v>37135</v>
+      </c>
+      <c r="L60" t="s">
+        <v>228</v>
+      </c>
+      <c r="M60">
+        <v>13</v>
+      </c>
+      <c r="N60">
+        <v>35.911769</v>
+      </c>
+      <c r="O60">
+        <v>-79.050968999999995</v>
+      </c>
+      <c r="P60">
+        <v>20500</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>93</v>
+      </c>
+      <c r="R60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <v>450</v>
+      </c>
+      <c r="T60" t="s">
+        <v>94</v>
+      </c>
+      <c r="U60" t="s">
+        <v>41</v>
+      </c>
+      <c r="V60" t="s">
+        <v>41</v>
+      </c>
+      <c r="W60">
+        <v>3704</v>
+      </c>
+      <c r="X60">
+        <v>37056</v>
+      </c>
+      <c r="Y60">
+        <v>37023</v>
+      </c>
+      <c r="Z60">
+        <v>2016</v>
+      </c>
+      <c r="AA60" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB60" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>-96.749709519999996</v>
+      </c>
+      <c r="B61">
+        <v>32.984678780000003</v>
+      </c>
+      <c r="C61">
+        <v>3792</v>
+      </c>
+      <c r="D61">
+        <v>228787</v>
+      </c>
+      <c r="E61" t="s">
+        <v>229</v>
+      </c>
+      <c r="F61" t="s">
+        <v>230</v>
+      </c>
+      <c r="G61" t="s">
+        <v>231</v>
+      </c>
+      <c r="H61" t="s">
+        <v>232</v>
+      </c>
+      <c r="I61" t="s">
+        <v>233</v>
+      </c>
+      <c r="J61">
+        <v>48</v>
+      </c>
+      <c r="K61">
+        <v>48113</v>
+      </c>
+      <c r="L61" t="s">
+        <v>234</v>
+      </c>
+      <c r="M61">
+        <v>12</v>
+      </c>
+      <c r="N61">
+        <v>32.984673000000001</v>
+      </c>
+      <c r="O61">
+        <v>-96.749701999999999</v>
+      </c>
+      <c r="P61">
+        <v>19100</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>235</v>
+      </c>
+      <c r="R61">
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <v>206</v>
+      </c>
+      <c r="T61" t="s">
+        <v>236</v>
+      </c>
+      <c r="U61" t="s">
+        <v>41</v>
+      </c>
+      <c r="V61" t="s">
+        <v>41</v>
+      </c>
+      <c r="W61">
+        <v>4832</v>
+      </c>
+      <c r="X61">
+        <v>48102</v>
+      </c>
+      <c r="Y61">
+        <v>48008</v>
+      </c>
+      <c r="Z61">
+        <v>2016</v>
+      </c>
+      <c r="AA61" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB61" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>-122.31312990000001</v>
+      </c>
+      <c r="B62">
+        <v>47.656218619999997</v>
+      </c>
+      <c r="C62">
+        <v>4034</v>
+      </c>
+      <c r="D62">
+        <v>236948</v>
+      </c>
+      <c r="E62" t="s">
+        <v>237</v>
+      </c>
+      <c r="F62" t="s">
+        <v>238</v>
+      </c>
+      <c r="G62" t="s">
+        <v>239</v>
+      </c>
+      <c r="H62" t="s">
+        <v>240</v>
+      </c>
+      <c r="I62" t="s">
+        <v>241</v>
+      </c>
+      <c r="J62">
+        <v>53</v>
+      </c>
+      <c r="K62">
+        <v>53033</v>
+      </c>
+      <c r="L62" t="s">
+        <v>242</v>
+      </c>
+      <c r="M62">
+        <v>11</v>
+      </c>
+      <c r="N62">
+        <v>47.656213000000001</v>
+      </c>
+      <c r="O62">
+        <v>-122.313115</v>
+      </c>
+      <c r="P62">
+        <v>42660</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>243</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>500</v>
+      </c>
+      <c r="T62" t="s">
+        <v>244</v>
+      </c>
+      <c r="U62" t="s">
+        <v>41</v>
+      </c>
+      <c r="V62" t="s">
+        <v>41</v>
+      </c>
+      <c r="W62">
+        <v>5307</v>
+      </c>
+      <c r="X62">
+        <v>53043</v>
+      </c>
+      <c r="Y62">
+        <v>53043</v>
+      </c>
+      <c r="Z62">
+        <v>2016</v>
+      </c>
+      <c r="AA62" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB62" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>-88.230314759999999</v>
+      </c>
+      <c r="B63">
+        <v>40.10887151</v>
+      </c>
+      <c r="C63">
+        <v>1046</v>
+      </c>
+      <c r="D63">
+        <v>145637</v>
+      </c>
+      <c r="E63" t="s">
+        <v>155</v>
+      </c>
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+      <c r="G63" t="s">
+        <v>157</v>
+      </c>
+      <c r="H63" t="s">
+        <v>53</v>
+      </c>
+      <c r="I63" t="s">
+        <v>158</v>
+      </c>
+      <c r="J63">
+        <v>17</v>
+      </c>
+      <c r="K63">
+        <v>17019</v>
+      </c>
+      <c r="L63" t="s">
+        <v>159</v>
+      </c>
+      <c r="M63">
+        <v>13</v>
+      </c>
+      <c r="N63">
+        <v>40.108863999999997</v>
+      </c>
+      <c r="O63">
+        <v>-88.230309000000005</v>
+      </c>
+      <c r="P63">
+        <v>16580</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>160</v>
+      </c>
+      <c r="R63">
+        <v>1</v>
+      </c>
+      <c r="S63" t="s">
+        <v>41</v>
+      </c>
+      <c r="T63" t="s">
+        <v>41</v>
+      </c>
+      <c r="U63" t="s">
+        <v>41</v>
+      </c>
+      <c r="V63" t="s">
+        <v>41</v>
+      </c>
+      <c r="W63">
+        <v>1713</v>
+      </c>
+      <c r="X63">
+        <v>17103</v>
+      </c>
+      <c r="Y63">
+        <v>17052</v>
+      </c>
+      <c r="Z63">
+        <v>2016</v>
+      </c>
+      <c r="AA63" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>-122.31312990000001</v>
+      </c>
+      <c r="B64">
+        <v>47.656218619999997</v>
+      </c>
+      <c r="C64">
+        <v>4034</v>
+      </c>
+      <c r="D64">
+        <v>236948</v>
+      </c>
+      <c r="E64" t="s">
+        <v>237</v>
+      </c>
+      <c r="F64" t="s">
+        <v>238</v>
+      </c>
+      <c r="G64" t="s">
+        <v>239</v>
+      </c>
+      <c r="H64" t="s">
+        <v>240</v>
+      </c>
+      <c r="I64" t="s">
+        <v>241</v>
+      </c>
+      <c r="J64">
+        <v>53</v>
+      </c>
+      <c r="K64">
+        <v>53033</v>
+      </c>
+      <c r="L64" t="s">
+        <v>242</v>
+      </c>
+      <c r="M64">
+        <v>11</v>
+      </c>
+      <c r="N64">
+        <v>47.656213000000001</v>
+      </c>
+      <c r="O64">
+        <v>-122.313115</v>
+      </c>
+      <c r="P64">
+        <v>42660</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>243</v>
+      </c>
+      <c r="R64">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <v>500</v>
+      </c>
+      <c r="T64" t="s">
+        <v>244</v>
+      </c>
+      <c r="U64" t="s">
+        <v>41</v>
+      </c>
+      <c r="V64" t="s">
+        <v>41</v>
+      </c>
+      <c r="W64">
+        <v>5307</v>
+      </c>
+      <c r="X64">
+        <v>53043</v>
+      </c>
+      <c r="Y64">
+        <v>53043</v>
+      </c>
+      <c r="Z64">
+        <v>2016</v>
+      </c>
+      <c r="AA64" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB64" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>-79.050971739999994</v>
+      </c>
+      <c r="B65">
+        <v>35.911776089999996</v>
+      </c>
+      <c r="C65">
+        <v>2731</v>
+      </c>
+      <c r="D65">
+        <v>199120</v>
+      </c>
+      <c r="E65" t="s">
+        <v>225</v>
+      </c>
+      <c r="F65" t="s">
+        <v>226</v>
+      </c>
+      <c r="G65" t="s">
+        <v>227</v>
+      </c>
+      <c r="H65" t="s">
+        <v>91</v>
+      </c>
+      <c r="I65">
+        <v>27599</v>
+      </c>
+      <c r="J65">
+        <v>37</v>
+      </c>
+      <c r="K65">
+        <v>37135</v>
+      </c>
+      <c r="L65" t="s">
+        <v>228</v>
+      </c>
+      <c r="M65">
+        <v>13</v>
+      </c>
+      <c r="N65">
+        <v>35.911769</v>
+      </c>
+      <c r="O65">
+        <v>-79.050968999999995</v>
+      </c>
+      <c r="P65">
+        <v>20500</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>93</v>
+      </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <v>450</v>
+      </c>
+      <c r="T65" t="s">
+        <v>94</v>
+      </c>
+      <c r="U65" t="s">
+        <v>41</v>
+      </c>
+      <c r="V65" t="s">
+        <v>41</v>
+      </c>
+      <c r="W65">
+        <v>3704</v>
+      </c>
+      <c r="X65">
+        <v>37056</v>
+      </c>
+      <c r="Y65">
+        <v>37023</v>
+      </c>
+      <c r="Z65">
+        <v>2016</v>
+      </c>
+      <c r="AA65" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB65" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>-86.526909180000004</v>
+      </c>
+      <c r="B66">
+        <v>39.16639043</v>
+      </c>
+      <c r="C66">
+        <v>1198</v>
+      </c>
+      <c r="D66">
+        <v>151351</v>
+      </c>
+      <c r="E66" t="s">
+        <v>246</v>
+      </c>
+      <c r="F66" t="s">
+        <v>247</v>
+      </c>
+      <c r="G66" t="s">
+        <v>248</v>
+      </c>
+      <c r="H66" t="s">
+        <v>147</v>
+      </c>
+      <c r="I66" t="s">
+        <v>249</v>
+      </c>
+      <c r="J66">
+        <v>18</v>
+      </c>
+      <c r="K66">
+        <v>18105</v>
+      </c>
+      <c r="L66" t="s">
+        <v>250</v>
+      </c>
+      <c r="M66">
+        <v>13</v>
+      </c>
+      <c r="N66">
+        <v>39.166383000000003</v>
+      </c>
+      <c r="O66">
+        <v>-86.526904000000002</v>
+      </c>
+      <c r="P66">
+        <v>14020</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>251</v>
+      </c>
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <v>144</v>
+      </c>
+      <c r="T66" t="s">
+        <v>252</v>
+      </c>
+      <c r="U66" t="s">
+        <v>41</v>
+      </c>
+      <c r="V66" t="s">
+        <v>41</v>
+      </c>
+      <c r="W66">
+        <v>1809</v>
+      </c>
+      <c r="X66">
+        <v>18061</v>
+      </c>
+      <c r="Y66">
+        <v>18040</v>
+      </c>
+      <c r="Z66">
+        <v>2016</v>
+      </c>
+      <c r="AA66" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>-76.136977290000004</v>
+      </c>
+      <c r="B67">
+        <v>43.040184619999998</v>
+      </c>
+      <c r="C67">
+        <v>2616</v>
+      </c>
+      <c r="D67">
+        <v>196413</v>
+      </c>
+      <c r="E67" t="s">
+        <v>254</v>
+      </c>
+      <c r="F67" t="s">
+        <v>255</v>
+      </c>
+      <c r="G67" t="s">
+        <v>256</v>
+      </c>
+      <c r="H67" t="s">
+        <v>60</v>
+      </c>
+      <c r="I67">
+        <v>13244</v>
+      </c>
+      <c r="J67">
+        <v>36</v>
+      </c>
+      <c r="K67">
+        <v>36067</v>
+      </c>
+      <c r="L67" t="s">
+        <v>257</v>
+      </c>
+      <c r="M67">
+        <v>12</v>
+      </c>
+      <c r="N67">
+        <v>43.040176000000002</v>
+      </c>
+      <c r="O67">
+        <v>-76.136975000000007</v>
+      </c>
+      <c r="P67">
+        <v>45060</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>258</v>
+      </c>
+      <c r="R67">
+        <v>1</v>
+      </c>
+      <c r="S67">
+        <v>532</v>
+      </c>
+      <c r="T67" t="s">
+        <v>259</v>
+      </c>
+      <c r="U67" t="s">
+        <v>41</v>
+      </c>
+      <c r="V67" t="s">
+        <v>41</v>
+      </c>
+      <c r="W67">
+        <v>3624</v>
+      </c>
+      <c r="X67">
+        <v>36129</v>
+      </c>
+      <c r="Y67">
+        <v>36053</v>
+      </c>
+      <c r="Z67">
+        <v>2016</v>
+      </c>
+      <c r="AA67" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>-71.118313610000001</v>
+      </c>
+      <c r="B68">
+        <v>42.374479669999999</v>
+      </c>
+      <c r="C68">
+        <v>1678</v>
+      </c>
+      <c r="D68">
+        <v>166027</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G68" t="s">
+        <v>44</v>
+      </c>
+      <c r="H68" t="s">
+        <v>45</v>
+      </c>
+      <c r="I68">
+        <v>2138</v>
+      </c>
+      <c r="J68">
+        <v>25</v>
+      </c>
+      <c r="K68">
+        <v>25017</v>
+      </c>
+      <c r="L68" t="s">
+        <v>46</v>
+      </c>
+      <c r="M68">
+        <v>12</v>
+      </c>
+      <c r="N68">
+        <v>42.374471</v>
+      </c>
+      <c r="O68">
+        <v>-71.118313000000001</v>
+      </c>
+      <c r="P68">
+        <v>14460</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>47</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="S68">
+        <v>148</v>
+      </c>
+      <c r="T68" t="s">
+        <v>48</v>
+      </c>
+      <c r="U68">
+        <v>71650</v>
+      </c>
+      <c r="V68" t="s">
+        <v>49</v>
+      </c>
+      <c r="W68">
+        <v>2505</v>
+      </c>
+      <c r="X68">
+        <v>25142</v>
+      </c>
+      <c r="Y68">
+        <v>25026</v>
+      </c>
+      <c r="Z68">
+        <v>2016</v>
+      </c>
+      <c r="AA68" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB68" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>-118.28418120000001</v>
+      </c>
+      <c r="B69">
+        <v>34.021285849999998</v>
+      </c>
+      <c r="C69">
+        <v>536</v>
+      </c>
+      <c r="D69">
+        <v>123961</v>
+      </c>
+      <c r="E69" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" t="s">
+        <v>153</v>
+      </c>
+      <c r="G69" t="s">
+        <v>154</v>
+      </c>
+      <c r="H69" t="s">
+        <v>37</v>
+      </c>
+      <c r="I69">
+        <v>90089</v>
+      </c>
+      <c r="J69">
+        <v>6</v>
+      </c>
+      <c r="K69">
+        <v>6037</v>
+      </c>
+      <c r="L69" t="s">
+        <v>133</v>
+      </c>
+      <c r="M69">
+        <v>11</v>
+      </c>
+      <c r="N69">
+        <v>34.021281000000002</v>
+      </c>
+      <c r="O69">
+        <v>-118.28416900000001</v>
+      </c>
+      <c r="P69">
+        <v>31080</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>134</v>
+      </c>
+      <c r="R69">
+        <v>1</v>
+      </c>
+      <c r="S69">
+        <v>348</v>
+      </c>
+      <c r="T69" t="s">
+        <v>135</v>
+      </c>
+      <c r="U69" t="s">
+        <v>41</v>
+      </c>
+      <c r="V69" t="s">
+        <v>41</v>
+      </c>
+      <c r="W69">
+        <v>637</v>
+      </c>
+      <c r="X69">
+        <v>6059</v>
+      </c>
+      <c r="Y69">
+        <v>6030</v>
+      </c>
+      <c r="Z69">
+        <v>2016</v>
+      </c>
+      <c r="AA69" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB69" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>-71.0921156</v>
+      </c>
+      <c r="B70">
+        <v>42.360103670000001</v>
+      </c>
+      <c r="C70">
+        <v>1700</v>
+      </c>
+      <c r="D70">
+        <v>166683</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G70" t="s">
+        <v>44</v>
+      </c>
+      <c r="H70" t="s">
+        <v>45</v>
+      </c>
+      <c r="I70" t="s">
+        <v>114</v>
+      </c>
+      <c r="J70">
+        <v>25</v>
+      </c>
+      <c r="K70">
+        <v>25017</v>
+      </c>
+      <c r="L70" t="s">
+        <v>46</v>
+      </c>
+      <c r="M70">
+        <v>12</v>
+      </c>
+      <c r="N70">
+        <v>42.360095000000001</v>
+      </c>
+      <c r="O70">
+        <v>-71.092115000000007</v>
+      </c>
+      <c r="P70">
+        <v>14460</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>47</v>
+      </c>
+      <c r="R70">
+        <v>1</v>
+      </c>
+      <c r="S70">
+        <v>148</v>
+      </c>
+      <c r="T70" t="s">
+        <v>48</v>
+      </c>
+      <c r="U70">
+        <v>71650</v>
+      </c>
+      <c r="V70" t="s">
+        <v>49</v>
+      </c>
+      <c r="W70">
+        <v>2507</v>
+      </c>
+      <c r="X70">
+        <v>25191</v>
+      </c>
+      <c r="Y70">
+        <v>25027</v>
+      </c>
+      <c r="Z70">
+        <v>2016</v>
+      </c>
+      <c r="AA70" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>-122.1644471</v>
+      </c>
+      <c r="B71">
+        <v>37.429536929999998</v>
+      </c>
+      <c r="C71">
+        <v>4248</v>
+      </c>
+      <c r="D71">
+        <v>243744</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G71" t="s">
+        <v>36</v>
+      </c>
+      <c r="H71" t="s">
+        <v>37</v>
+      </c>
+      <c r="I71">
+        <v>94305</v>
+      </c>
+      <c r="J71">
+        <v>6</v>
+      </c>
+      <c r="K71">
+        <v>6085</v>
+      </c>
+      <c r="L71" t="s">
+        <v>38</v>
+      </c>
+      <c r="M71">
+        <v>21</v>
+      </c>
+      <c r="N71">
+        <v>37.429532000000002</v>
+      </c>
+      <c r="O71">
+        <v>-122.164434</v>
+      </c>
+      <c r="P71">
+        <v>41940</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>39</v>
+      </c>
+      <c r="R71">
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <v>488</v>
+      </c>
+      <c r="T71" t="s">
+        <v>40</v>
+      </c>
+      <c r="U71" t="s">
+        <v>41</v>
+      </c>
+      <c r="V71" t="s">
+        <v>41</v>
+      </c>
+      <c r="W71">
+        <v>618</v>
+      </c>
+      <c r="X71">
+        <v>6024</v>
+      </c>
+      <c r="Y71">
+        <v>6013</v>
+      </c>
+      <c r="Z71">
+        <v>2016</v>
+      </c>
+      <c r="AA71" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>-122.2604762</v>
+      </c>
+      <c r="B72">
+        <v>37.871922959999999</v>
+      </c>
+      <c r="C72">
+        <v>247</v>
+      </c>
+      <c r="D72">
+        <v>110635</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G72" t="s">
+        <v>102</v>
+      </c>
+      <c r="H72" t="s">
+        <v>37</v>
+      </c>
+      <c r="I72">
+        <v>94720</v>
+      </c>
+      <c r="J72">
+        <v>6</v>
+      </c>
+      <c r="K72">
+        <v>6001</v>
+      </c>
+      <c r="L72" t="s">
+        <v>103</v>
+      </c>
+      <c r="M72">
+        <v>12</v>
+      </c>
+      <c r="N72">
+        <v>37.871918000000001</v>
+      </c>
+      <c r="O72">
+        <v>-122.260463</v>
+      </c>
+      <c r="P72">
+        <v>41860</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>104</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72">
+        <v>488</v>
+      </c>
+      <c r="T72" t="s">
+        <v>40</v>
+      </c>
+      <c r="U72" t="s">
+        <v>41</v>
+      </c>
+      <c r="V72" t="s">
+        <v>41</v>
+      </c>
+      <c r="W72">
+        <v>613</v>
+      </c>
+      <c r="X72">
+        <v>6015</v>
+      </c>
+      <c r="Y72">
+        <v>6009</v>
+      </c>
+      <c r="Z72">
+        <v>2016</v>
+      </c>
+      <c r="AA72" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>-76.944723269999997</v>
+      </c>
+      <c r="B73">
+        <v>38.988185809999997</v>
+      </c>
+      <c r="C73">
+        <v>1595</v>
+      </c>
+      <c r="D73">
+        <v>163286</v>
+      </c>
+      <c r="E73" t="s">
+        <v>261</v>
+      </c>
+      <c r="F73" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" t="s">
+        <v>262</v>
+      </c>
+      <c r="H73" t="s">
+        <v>167</v>
+      </c>
+      <c r="I73">
+        <v>20742</v>
+      </c>
+      <c r="J73">
+        <v>24</v>
+      </c>
+      <c r="K73">
+        <v>24033</v>
+      </c>
+      <c r="L73" t="s">
+        <v>263</v>
+      </c>
+      <c r="M73">
+        <v>21</v>
+      </c>
+      <c r="N73">
+        <v>38.988177999999998</v>
+      </c>
+      <c r="O73">
+        <v>-76.944721000000001</v>
+      </c>
+      <c r="P73">
+        <v>47900</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>264</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73">
+        <v>548</v>
+      </c>
+      <c r="T73" t="s">
+        <v>171</v>
+      </c>
+      <c r="U73" t="s">
+        <v>41</v>
+      </c>
+      <c r="V73" t="s">
+        <v>41</v>
+      </c>
+      <c r="W73">
+        <v>2405</v>
+      </c>
+      <c r="X73">
+        <v>24021</v>
+      </c>
+      <c r="Y73">
+        <v>24021</v>
+      </c>
+      <c r="Z73">
+        <v>2016</v>
+      </c>
+      <c r="AA73" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>-73.825015519999994</v>
+      </c>
+      <c r="B74">
+        <v>42.686925639999998</v>
+      </c>
+      <c r="C74">
+        <v>2592</v>
+      </c>
+      <c r="D74">
+        <v>196060</v>
+      </c>
+      <c r="E74" t="s">
+        <v>266</v>
+      </c>
+      <c r="F74" t="s">
+        <v>267</v>
+      </c>
+      <c r="G74" t="s">
+        <v>268</v>
+      </c>
+      <c r="H74" t="s">
+        <v>60</v>
+      </c>
+      <c r="I74">
+        <v>12222</v>
+      </c>
+      <c r="J74">
+        <v>36</v>
+      </c>
+      <c r="K74">
+        <v>36001</v>
+      </c>
+      <c r="L74" t="s">
+        <v>269</v>
+      </c>
+      <c r="M74">
+        <v>13</v>
+      </c>
+      <c r="N74">
+        <v>42.686917000000001</v>
+      </c>
+      <c r="O74">
+        <v>-73.825013999999996</v>
+      </c>
+      <c r="P74">
+        <v>10580</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>270</v>
+      </c>
+      <c r="R74">
+        <v>1</v>
+      </c>
+      <c r="S74">
+        <v>104</v>
+      </c>
+      <c r="T74" t="s">
+        <v>271</v>
+      </c>
+      <c r="U74" t="s">
+        <v>41</v>
+      </c>
+      <c r="V74" t="s">
+        <v>41</v>
+      </c>
+      <c r="W74">
+        <v>3620</v>
+      </c>
+      <c r="X74">
+        <v>36109</v>
+      </c>
+      <c r="Y74">
+        <v>36044</v>
+      </c>
+      <c r="Z74">
+        <v>2016</v>
+      </c>
+      <c r="AA74" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB74" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>